<commit_message>
updated excel files. Vgps are calculated from paleomag direction when slat and slong where reported, otherwise, we take the vgp coordinates
</commit_message>
<xml_diff>
--- a/data/VGPs_NAM/11.xlsx
+++ b/data/VGPs_NAM/11.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mjNDla0rMaJQK0G5tO+910++cyEIg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mjR5hN9kD3WdzAIkP/O4bjFxNl4Og=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="59">
   <si>
     <t>Study level data</t>
   </si>
@@ -83,6 +83,9 @@
     <t>age</t>
   </si>
   <si>
+    <t>2_sigma</t>
+  </si>
+  <si>
     <t>min_age</t>
   </si>
   <si>
@@ -116,7 +119,10 @@
     <t>Tauxe et al. (2004)</t>
   </si>
   <si>
-    <t>Ar/Ar ages of 0.1 to 5.78 Ma</t>
+    <t>Ar/Ar ages of 0.1 to 5.75 Ma</t>
+  </si>
+  <si>
+    <t>Plateau, TFA and isochron ages available</t>
   </si>
   <si>
     <t>Site level data</t>
@@ -154,6 +160,9 @@
     <t>sr01</t>
   </si>
   <si>
+    <t>plateau age</t>
+  </si>
+  <si>
     <t>sr03</t>
   </si>
   <si>
@@ -227,7 +236,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -238,6 +247,11 @@
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <color theme="1"/>
     </font>
     <font>
       <sz val="12.0"/>
@@ -251,11 +265,20 @@
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="12.0"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -266,6 +289,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF00FF"/>
         <bgColor rgb="FFFF00FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="0"/>
       </patternFill>
     </fill>
   </fills>
@@ -295,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -303,37 +332,58 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="2" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="2" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
+    <xf borderId="2" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
     <xf borderId="2" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="2" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="2" fillId="3" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="2" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -550,7 +600,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="30" width="9.38"/>
+    <col customWidth="1" min="1" max="31" width="9.38"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -604,7 +654,7 @@
       <c r="O2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="3" t="s">
         <v>16</v>
       </c>
       <c r="Q2" s="2" t="s">
@@ -625,73 +675,80 @@
       <c r="V2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="W2" s="2" t="s">
         <v>23</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="5">
+      <c r="A3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="6">
         <v>42.86</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="6">
         <v>247.9</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="7">
         <v>23.0</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="7">
         <v>38.2</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="7">
         <v>5.0</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="8">
         <v>-86.9</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="9">
         <v>187.8</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K3" s="7">
         <v>24.8</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="7">
         <v>6.2</v>
       </c>
-      <c r="M3" s="9">
+      <c r="M3" s="10">
         <v>6.2</v>
       </c>
-      <c r="N3" s="6">
+      <c r="N3" s="7">
         <v>6.2</v>
       </c>
-      <c r="O3" s="10">
+      <c r="O3" s="11">
         <v>3.0</v>
       </c>
-      <c r="P3" s="5">
+      <c r="P3" s="12"/>
+      <c r="Q3" s="6">
         <v>0.0</v>
       </c>
-      <c r="Q3" s="5">
+      <c r="R3" s="6">
         <v>6.0</v>
       </c>
-      <c r="S3" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="T3" s="6">
+      <c r="T3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="U3" s="7">
         <v>5.0</v>
       </c>
-      <c r="U3" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="V3" s="11" t="s">
+      <c r="V3" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="Y3" s="2"/>
+      <c r="W3" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="X3" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z3" s="2"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6">
@@ -705,7 +762,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>5</v>
@@ -717,13 +774,13 @@
         <v>7</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>11</v>
@@ -740,7 +797,7 @@
       <c r="O6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="P6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="Q6" s="2" t="s">
@@ -761,813 +818,1085 @@
       <c r="V6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="W6" s="3" t="s">
+      <c r="W6" s="2" t="s">
         <v>23</v>
+      </c>
+      <c r="X6" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="12">
+      <c r="A7" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="15">
         <v>42.60264</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="15">
         <v>245.60245</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="16">
         <v>8.0</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="15">
         <v>330.1</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="15">
         <v>64.9</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="15">
         <v>581.5</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="15">
         <v>2.3</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="15">
         <v>68.6</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="15">
         <v>47.2</v>
       </c>
-      <c r="S7" s="12" t="s">
-        <v>25</v>
+      <c r="N7" s="17"/>
+      <c r="O7" s="18">
+        <v>3.4</v>
+      </c>
+      <c r="P7" s="18">
+        <v>0.06</v>
+      </c>
+      <c r="T7" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="V7" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="X7" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="12">
+      <c r="A8" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="15">
         <v>42.60352</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="15">
         <v>245.5993</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="16">
         <v>7.0</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="15">
         <v>151.8</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="15">
         <v>57.5</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="15">
         <v>405.3</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="15">
         <v>3.0</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="15">
         <v>68.2</v>
       </c>
-      <c r="J8" s="12">
+      <c r="J8" s="15">
         <v>202.1</v>
       </c>
-      <c r="S8" s="12" t="s">
-        <v>25</v>
+      <c r="N8" s="17"/>
+      <c r="O8" s="18">
+        <v>2.0</v>
+      </c>
+      <c r="P8" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="T8" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="V8" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="X8" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="12">
+      <c r="A9" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="15">
         <v>42.60104</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="15">
         <v>245.59638</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="16">
         <v>5.0</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="15">
         <v>16.5</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="15">
         <v>54.6</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="15">
         <v>316.1</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="15">
         <v>4.3</v>
       </c>
-      <c r="I9" s="12">
+      <c r="I9" s="15">
         <v>75.1</v>
       </c>
-      <c r="J9" s="12">
+      <c r="J9" s="15">
         <v>229.5</v>
       </c>
-      <c r="S9" s="12" t="s">
-        <v>25</v>
+      <c r="N9" s="17"/>
+      <c r="O9" s="18">
+        <v>0.095</v>
+      </c>
+      <c r="P9" s="18">
+        <v>0.01</v>
+      </c>
+      <c r="T9" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="V9" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="X9" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="15">
+        <v>42.73656</v>
+      </c>
+      <c r="C10" s="15">
+        <v>245.16456</v>
+      </c>
+      <c r="D10" s="16">
+        <v>7.0</v>
+      </c>
+      <c r="E10" s="15">
+        <v>14.6</v>
+      </c>
+      <c r="F10" s="15">
+        <v>77.9</v>
+      </c>
+      <c r="G10" s="15">
+        <v>410.5</v>
+      </c>
+      <c r="H10" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="I10" s="15">
+        <v>63.6</v>
+      </c>
+      <c r="J10" s="15">
+        <v>125.5</v>
+      </c>
+      <c r="N10" s="17"/>
+      <c r="O10" s="18">
+        <v>0.395</v>
+      </c>
+      <c r="P10" s="18">
+        <v>0.02</v>
+      </c>
+      <c r="T10" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="V10" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="X10" s="15" t="s">
         <v>36</v>
-      </c>
-      <c r="B10" s="12">
-        <v>42.73656</v>
-      </c>
-      <c r="C10" s="12">
-        <v>245.16456</v>
-      </c>
-      <c r="D10" s="13">
-        <v>7.0</v>
-      </c>
-      <c r="E10" s="12">
-        <v>14.6</v>
-      </c>
-      <c r="F10" s="12">
-        <v>77.9</v>
-      </c>
-      <c r="G10" s="12">
-        <v>410.5</v>
-      </c>
-      <c r="H10" s="12">
-        <v>3.0</v>
-      </c>
-      <c r="I10" s="12">
-        <v>63.6</v>
-      </c>
-      <c r="J10" s="12">
-        <v>125.5</v>
-      </c>
-      <c r="S10" s="12" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="12">
+      <c r="A11" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="15">
         <v>42.8418</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="15">
         <v>245.11175</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="16">
         <v>7.0</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="15">
         <v>346.5</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="15">
         <v>73.7</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="15">
         <v>430.3</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="15">
         <v>3.0</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I11" s="15">
         <v>71.2</v>
       </c>
-      <c r="J11" s="12">
+      <c r="J11" s="15">
         <v>93.4</v>
       </c>
-      <c r="S11" s="12" t="s">
-        <v>25</v>
+      <c r="N11" s="17"/>
+      <c r="O11" s="18">
+        <v>0.373</v>
+      </c>
+      <c r="P11" s="18">
+        <v>0.01</v>
+      </c>
+      <c r="T11" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="V11" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="X11" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="12">
+      <c r="A12" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="15">
         <v>42.8657</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="15">
         <v>245.12742</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="16">
         <v>5.0</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="15">
         <v>15.3</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="15">
         <v>44.8</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="15">
         <v>227.6</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="15">
         <v>5.1</v>
       </c>
-      <c r="I12" s="12">
+      <c r="I12" s="15">
         <v>69.4</v>
       </c>
-      <c r="J12" s="12">
+      <c r="J12" s="15">
         <v>252.7</v>
       </c>
-      <c r="S12" s="12" t="s">
-        <v>25</v>
+      <c r="N12" s="17"/>
+      <c r="O12" s="18">
+        <v>0.404</v>
+      </c>
+      <c r="P12" s="18">
+        <v>0.01</v>
+      </c>
+      <c r="T12" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="V12" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="X12" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="12">
+      <c r="A13" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="15">
         <v>42.88822</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="15">
         <v>244.92279</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="16">
         <v>7.0</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="15">
         <v>347.4</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13" s="15">
         <v>65.6</v>
       </c>
-      <c r="G13" s="12">
+      <c r="G13" s="15">
         <v>227.9</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="15">
         <v>4.0</v>
       </c>
-      <c r="I13" s="12">
+      <c r="I13" s="15">
         <v>79.9</v>
       </c>
-      <c r="J13" s="12">
+      <c r="J13" s="15">
         <v>58.2</v>
       </c>
-      <c r="S13" s="12" t="s">
-        <v>25</v>
+      <c r="N13" s="17"/>
+      <c r="O13" s="18">
+        <v>0.052</v>
+      </c>
+      <c r="P13" s="18">
+        <v>0.02</v>
+      </c>
+      <c r="T13" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="V13" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="X13" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="12">
+      <c r="A14" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="15">
         <v>42.56857</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="15">
         <v>245.70095</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="16">
         <v>4.0</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="15">
         <v>169.3</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="15">
         <v>63.5</v>
       </c>
-      <c r="G14" s="12">
+      <c r="G14" s="15">
         <v>1197.9</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H14" s="15">
         <v>2.7</v>
       </c>
-      <c r="I14" s="12">
+      <c r="I14" s="15">
         <v>81.9</v>
       </c>
-      <c r="J14" s="12">
+      <c r="J14" s="15">
         <v>226.0</v>
       </c>
-      <c r="S14" s="12" t="s">
-        <v>25</v>
+      <c r="N14" s="17"/>
+      <c r="O14" s="18">
+        <v>1.76</v>
+      </c>
+      <c r="P14" s="18">
+        <v>0.32</v>
+      </c>
+      <c r="T14" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="V14" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="X14" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="12">
+      <c r="A15" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="15">
         <v>42.49962</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="15">
         <v>245.85094</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15" s="16">
         <v>5.0</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="15">
         <v>172.4</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F15" s="15">
         <v>66.9</v>
       </c>
-      <c r="G15" s="12">
+      <c r="G15" s="15">
         <v>797.1</v>
       </c>
-      <c r="H15" s="12">
+      <c r="H15" s="15">
         <v>2.7</v>
       </c>
-      <c r="I15" s="12">
+      <c r="I15" s="15">
         <v>81.2</v>
       </c>
-      <c r="J15" s="12">
+      <c r="J15" s="15">
         <v>259.9</v>
       </c>
-      <c r="S15" s="12" t="s">
-        <v>25</v>
+      <c r="N15" s="17"/>
+      <c r="O15" s="18">
+        <v>1.69</v>
+      </c>
+      <c r="P15" s="18">
+        <v>0.04</v>
+      </c>
+      <c r="T15" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="V15" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="X15" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="12">
+      <c r="A16" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="15">
         <v>42.50001</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16" s="15">
         <v>245.84971</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="16">
         <v>7.0</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="15">
         <v>6.3</v>
       </c>
-      <c r="F16" s="12">
+      <c r="F16" s="15">
         <v>29.7</v>
       </c>
-      <c r="G16" s="12">
+      <c r="G16" s="15">
         <v>335.5</v>
       </c>
-      <c r="H16" s="12">
+      <c r="H16" s="15">
         <v>3.3</v>
       </c>
-      <c r="I16" s="12">
+      <c r="I16" s="15">
         <v>62.9</v>
       </c>
-      <c r="J16" s="12">
+      <c r="J16" s="15">
         <v>280.7</v>
       </c>
-      <c r="S16" s="12" t="s">
-        <v>25</v>
+      <c r="N16" s="17"/>
+      <c r="O16" s="18">
+        <v>0.591</v>
+      </c>
+      <c r="P16" s="18">
+        <v>0.03</v>
+      </c>
+      <c r="T16" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="V16" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="X16" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="12">
+      <c r="A17" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="15">
         <v>42.52872</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="15">
         <v>245.97898</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="16">
         <v>6.0</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="15">
         <v>14.0</v>
       </c>
-      <c r="F17" s="12">
+      <c r="F17" s="15">
         <v>46.6</v>
       </c>
-      <c r="G17" s="12">
+      <c r="G17" s="15">
         <v>565.0</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H17" s="15">
         <v>2.9</v>
       </c>
-      <c r="I17" s="12">
+      <c r="I17" s="15">
         <v>71.5</v>
       </c>
-      <c r="J17" s="12">
+      <c r="J17" s="15">
         <v>251.8</v>
       </c>
-      <c r="S17" s="12" t="s">
-        <v>25</v>
+      <c r="N17" s="17"/>
+      <c r="O17" s="18">
+        <v>0.291</v>
+      </c>
+      <c r="P17" s="18">
+        <v>0.03</v>
+      </c>
+      <c r="T17" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="V17" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="X17" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="12">
+      <c r="A18" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="15">
         <v>42.45559</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C18" s="15">
         <v>245.63636</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18" s="16">
         <v>5.0</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="15">
         <v>163.3</v>
       </c>
-      <c r="F18" s="12">
+      <c r="F18" s="15">
         <v>62.2</v>
       </c>
-      <c r="G18" s="12">
+      <c r="G18" s="15">
         <v>325.8</v>
       </c>
-      <c r="H18" s="12">
+      <c r="H18" s="15">
         <v>4.2</v>
       </c>
-      <c r="I18" s="12">
+      <c r="I18" s="15">
         <v>77.8</v>
       </c>
-      <c r="J18" s="12">
+      <c r="J18" s="15">
         <v>214.8</v>
       </c>
-      <c r="S18" s="12" t="s">
-        <v>25</v>
+      <c r="N18" s="17"/>
+      <c r="O18" s="18">
+        <v>1.73</v>
+      </c>
+      <c r="P18" s="18">
+        <v>0.02</v>
+      </c>
+      <c r="T18" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="V18" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="X18" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" s="12">
+      <c r="A19" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="15">
         <v>42.48923</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19" s="15">
         <v>245.60009</v>
       </c>
-      <c r="D19" s="13">
+      <c r="D19" s="16">
         <v>5.0</v>
       </c>
-      <c r="E19" s="12">
+      <c r="E19" s="15">
         <v>2.9</v>
       </c>
-      <c r="F19" s="12">
+      <c r="F19" s="15">
         <v>61.9</v>
       </c>
-      <c r="G19" s="12">
+      <c r="G19" s="15">
         <v>871.8</v>
       </c>
-      <c r="H19" s="12">
+      <c r="H19" s="15">
         <v>2.6</v>
       </c>
-      <c r="I19" s="12">
+      <c r="I19" s="15">
         <v>87.8</v>
       </c>
-      <c r="J19" s="12">
+      <c r="J19" s="15">
         <v>186.9</v>
       </c>
-      <c r="S19" s="12" t="s">
-        <v>25</v>
+      <c r="N19" s="17"/>
+      <c r="O19" s="18">
+        <v>2.89</v>
+      </c>
+      <c r="P19" s="18">
+        <v>0.04</v>
+      </c>
+      <c r="T19" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="V19" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="X19" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B20" s="12">
+      <c r="A20" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="15">
         <v>42.46186</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C20" s="15">
         <v>245.61471</v>
       </c>
-      <c r="D20" s="13">
+      <c r="D20" s="16">
         <v>7.0</v>
       </c>
-      <c r="E20" s="12">
+      <c r="E20" s="15">
         <v>358.6</v>
       </c>
-      <c r="F20" s="12">
+      <c r="F20" s="15">
         <v>62.4</v>
       </c>
-      <c r="G20" s="12">
+      <c r="G20" s="15">
         <v>153.1</v>
       </c>
-      <c r="H20" s="12">
+      <c r="H20" s="15">
         <v>5.0</v>
       </c>
-      <c r="I20" s="12">
+      <c r="I20" s="15">
         <v>88.6</v>
       </c>
-      <c r="J20" s="12">
+      <c r="J20" s="15">
         <v>47.1</v>
       </c>
-      <c r="S20" s="12" t="s">
-        <v>25</v>
+      <c r="N20" s="17"/>
+      <c r="O20" s="18">
+        <v>2.94</v>
+      </c>
+      <c r="P20" s="18">
+        <v>0.05</v>
+      </c>
+      <c r="T20" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="V20" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="X20" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="B21" s="12">
+      <c r="A21" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="15">
         <v>42.65289</v>
       </c>
-      <c r="C21" s="12">
+      <c r="C21" s="15">
         <v>246.98823</v>
       </c>
-      <c r="D21" s="13">
+      <c r="D21" s="16">
         <v>7.0</v>
       </c>
-      <c r="E21" s="12">
+      <c r="E21" s="15">
         <v>195.8</v>
       </c>
-      <c r="F21" s="12">
+      <c r="F21" s="15">
         <v>50.6</v>
       </c>
-      <c r="G21" s="12">
+      <c r="G21" s="15">
         <v>535.2</v>
       </c>
-      <c r="H21" s="12">
+      <c r="H21" s="15">
         <v>2.6</v>
       </c>
-      <c r="I21" s="12">
+      <c r="I21" s="15">
         <v>72.7</v>
       </c>
-      <c r="J21" s="12">
+      <c r="J21" s="15">
         <v>60.1</v>
       </c>
-      <c r="S21" s="12" t="s">
-        <v>25</v>
+      <c r="N21" s="17"/>
+      <c r="O21" s="18">
+        <v>5.75</v>
+      </c>
+      <c r="P21" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="T21" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="V21" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="X21" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" s="12">
+      <c r="A22" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="15">
         <v>43.30504</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C22" s="15">
         <v>247.73219</v>
       </c>
-      <c r="D22" s="13">
+      <c r="D22" s="16">
         <v>8.0</v>
       </c>
-      <c r="E22" s="12">
+      <c r="E22" s="15">
         <v>9.4</v>
       </c>
-      <c r="F22" s="12">
+      <c r="F22" s="15">
         <v>62.7</v>
       </c>
-      <c r="G22" s="12">
+      <c r="G22" s="15">
         <v>1244.7</v>
       </c>
-      <c r="H22" s="12">
+      <c r="H22" s="15">
         <v>1.6</v>
       </c>
-      <c r="I22" s="12">
+      <c r="I22" s="15">
         <v>82.8</v>
       </c>
-      <c r="J22" s="12">
+      <c r="J22" s="15">
         <v>190.6</v>
       </c>
-      <c r="S22" s="12" t="s">
-        <v>25</v>
+      <c r="N22" s="17"/>
+      <c r="O22" s="18">
+        <v>0.18</v>
+      </c>
+      <c r="P22" s="18">
+        <v>0.028</v>
+      </c>
+      <c r="T22" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="V22" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="X22" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B23" s="12">
+      <c r="A23" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="15">
         <v>43.36817</v>
       </c>
-      <c r="C23" s="12">
+      <c r="C23" s="15">
         <v>247.3447</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D23" s="16">
         <v>7.0</v>
       </c>
-      <c r="E23" s="12">
+      <c r="E23" s="15">
         <v>7.5</v>
       </c>
-      <c r="F23" s="12">
+      <c r="F23" s="15">
         <v>66.7</v>
       </c>
-      <c r="G23" s="12">
+      <c r="G23" s="15">
         <v>488.6</v>
       </c>
-      <c r="H23" s="12">
+      <c r="H23" s="15">
         <v>2.7</v>
       </c>
-      <c r="I23" s="12">
+      <c r="I23" s="15">
         <v>81.9</v>
       </c>
-      <c r="J23" s="12">
+      <c r="J23" s="15">
         <v>144.3</v>
       </c>
-      <c r="S23" s="12" t="s">
-        <v>25</v>
+      <c r="N23" s="17"/>
+      <c r="O23" s="18">
+        <v>0.191</v>
+      </c>
+      <c r="P23" s="18">
+        <v>0.02</v>
+      </c>
+      <c r="T23" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="V23" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="X23" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="12">
+      <c r="A24" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="15">
         <v>43.42133</v>
       </c>
-      <c r="C24" s="12">
+      <c r="C24" s="15">
         <v>247.25587</v>
       </c>
-      <c r="D24" s="13">
+      <c r="D24" s="16">
         <v>8.0</v>
       </c>
-      <c r="E24" s="12">
+      <c r="E24" s="15">
         <v>23.2</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F24" s="15">
         <v>54.0</v>
       </c>
-      <c r="G24" s="12">
+      <c r="G24" s="15">
         <v>1836.2</v>
       </c>
-      <c r="H24" s="12">
+      <c r="H24" s="15">
         <v>1.3</v>
       </c>
-      <c r="I24" s="12">
+      <c r="I24" s="15">
         <v>69.7</v>
       </c>
-      <c r="J24" s="12">
+      <c r="J24" s="15">
         <v>221.1</v>
       </c>
-      <c r="S24" s="12" t="s">
-        <v>25</v>
+      <c r="N24" s="17"/>
+      <c r="O24" s="18">
+        <v>0.12</v>
+      </c>
+      <c r="P24" s="18">
+        <v>0.078</v>
+      </c>
+      <c r="T24" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="V24" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="X24" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" s="12">
+      <c r="A25" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="15">
         <v>43.8859</v>
       </c>
-      <c r="C25" s="12">
+      <c r="C25" s="15">
         <v>247.19945</v>
       </c>
-      <c r="D25" s="13">
+      <c r="D25" s="16">
         <v>8.0</v>
       </c>
-      <c r="E25" s="12">
+      <c r="E25" s="15">
         <v>205.4</v>
       </c>
-      <c r="F25" s="12">
+      <c r="F25" s="15">
         <v>48.9</v>
       </c>
-      <c r="G25" s="12">
+      <c r="G25" s="15">
         <v>564.7</v>
       </c>
-      <c r="H25" s="12">
+      <c r="H25" s="15">
         <v>2.4</v>
       </c>
-      <c r="I25" s="12">
+      <c r="I25" s="15">
         <v>65.9</v>
       </c>
-      <c r="J25" s="12">
+      <c r="J25" s="15">
         <v>49.0</v>
       </c>
-      <c r="S25" s="12" t="s">
-        <v>25</v>
+      <c r="N25" s="17"/>
+      <c r="O25" s="18">
+        <v>0.945</v>
+      </c>
+      <c r="P25" s="18">
+        <v>0.06</v>
+      </c>
+      <c r="T25" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="V25" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="X25" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="B26" s="12">
+      <c r="A26" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="15">
         <v>43.84273</v>
       </c>
-      <c r="C26" s="12">
+      <c r="C26" s="15">
         <v>247.30639</v>
       </c>
-      <c r="D26" s="13">
+      <c r="D26" s="16">
         <v>6.0</v>
       </c>
-      <c r="E26" s="12">
+      <c r="E26" s="15">
         <v>197.1</v>
       </c>
-      <c r="F26" s="12">
+      <c r="F26" s="15">
         <v>63.8</v>
       </c>
-      <c r="G26" s="12">
+      <c r="G26" s="15">
         <v>258.5</v>
       </c>
-      <c r="H26" s="12">
+      <c r="H26" s="15">
         <v>4.3</v>
       </c>
-      <c r="I26" s="12">
+      <c r="I26" s="15">
         <v>77.8</v>
       </c>
-      <c r="J26" s="12">
+      <c r="J26" s="15">
         <v>9.1</v>
       </c>
-      <c r="S26" s="12" t="s">
-        <v>25</v>
+      <c r="T26" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="V26" s="20" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B27" s="12">
+      <c r="A27" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="15">
         <v>43.53289</v>
       </c>
-      <c r="C27" s="12">
+      <c r="C27" s="15">
         <v>248.29368</v>
       </c>
-      <c r="D27" s="13">
+      <c r="D27" s="16">
         <v>5.0</v>
       </c>
-      <c r="E27" s="12">
+      <c r="E27" s="15">
         <v>175.6</v>
       </c>
-      <c r="F27" s="12">
+      <c r="F27" s="15">
         <v>53.9</v>
       </c>
-      <c r="G27" s="12">
+      <c r="G27" s="15">
         <v>150.4</v>
       </c>
-      <c r="H27" s="12">
+      <c r="H27" s="15">
         <v>6.4</v>
       </c>
-      <c r="I27" s="12">
+      <c r="I27" s="15">
         <v>80.3</v>
       </c>
-      <c r="J27" s="12">
+      <c r="J27" s="15">
         <v>130.1</v>
       </c>
-      <c r="S27" s="12" t="s">
-        <v>25</v>
+      <c r="T27" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="V27" s="20" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="B28" s="12">
+      <c r="A28" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="15">
         <v>43.57494</v>
       </c>
-      <c r="C28" s="12">
+      <c r="C28" s="15">
         <v>248.26583</v>
       </c>
-      <c r="D28" s="13">
+      <c r="D28" s="16">
         <v>6.0</v>
       </c>
-      <c r="E28" s="12">
+      <c r="E28" s="15">
         <v>187.3</v>
       </c>
-      <c r="F28" s="12">
+      <c r="F28" s="15">
         <v>47.7</v>
       </c>
-      <c r="G28" s="12">
+      <c r="G28" s="15">
         <v>167.5</v>
       </c>
-      <c r="H28" s="12">
+      <c r="H28" s="15">
         <v>5.3</v>
       </c>
-      <c r="I28" s="12">
+      <c r="I28" s="15">
         <v>74.1</v>
       </c>
-      <c r="J28" s="12">
+      <c r="J28" s="15">
         <v>87.5</v>
       </c>
-      <c r="S28" s="12" t="s">
-        <v>25</v>
+      <c r="T28" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="V28" s="20" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29" s="12">
+      <c r="A29" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="15">
         <v>44.15663</v>
       </c>
-      <c r="C29" s="12">
+      <c r="C29" s="15">
         <v>248.57442</v>
       </c>
-      <c r="D29" s="13">
+      <c r="D29" s="16">
         <v>5.0</v>
       </c>
-      <c r="E29" s="12">
+      <c r="E29" s="15">
         <v>192.9</v>
       </c>
-      <c r="F29" s="12">
+      <c r="F29" s="15">
         <v>60.7</v>
       </c>
-      <c r="G29" s="12">
+      <c r="G29" s="15">
         <v>328.1</v>
       </c>
-      <c r="H29" s="12">
+      <c r="H29" s="15">
         <v>4.2</v>
       </c>
-      <c r="I29" s="12">
+      <c r="I29" s="15">
         <v>80.3</v>
       </c>
-      <c r="J29" s="12">
+      <c r="J29" s="15">
         <v>31.5</v>
       </c>
-      <c r="S29" s="12" t="s">
-        <v>25</v>
+      <c r="N29" s="17"/>
+      <c r="O29" s="18">
+        <v>0.39</v>
+      </c>
+      <c r="P29" s="18">
+        <v>0.038</v>
+      </c>
+      <c r="T29" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="V29" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="X29" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1"/>

</xml_diff>